<commit_message>
Chapter 1 RU initial upload
</commit_message>
<xml_diff>
--- a/REVELATOR/.SRT/JP/NameKeywordList.xlsx
+++ b/REVELATOR/.SRT/JP/NameKeywordList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\GitHub\Guilty-Gear-SIGN-Ru-Translation\REVELATOR\.SRT\JP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2537EA-3B1A-417C-AE31-6A84FA443FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11872BAE-16E5-479B-A353-12A23BA40B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,12 +598,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="D71" authorId="0" shapeId="0" xr:uid="{27A4C684-13B7-4C5F-AAE0-44940873A0E8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://guiltygear.wiki.gg/wiki/Sacred_Order_of_Holy_Knights</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="397">
   <si>
     <t>Code</t>
   </si>
@@ -1902,12 +1916,21 @@
       <t>(отсылка на установку программ)</t>
     </r>
   </si>
+  <si>
+    <t>聖騎士団</t>
+  </si>
+  <si>
+    <t>Sacred Order of Holy Knights (Holy Order)</t>
+  </si>
+  <si>
+    <t>Священный Орден Святых Рыцарей (Священный Орден)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1976,6 +1999,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2241,8 +2271,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C42E803F-D6E1-435B-BCDD-7A3149C39A7A}" name="Таблица5" displayName="Таблица5" ref="B2:E70" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B2:E70" xr:uid="{C42E803F-D6E1-435B-BCDD-7A3149C39A7A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C42E803F-D6E1-435B-BCDD-7A3149C39A7A}" name="Таблица5" displayName="Таблица5" ref="B2:E71" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="B2:E71" xr:uid="{C42E803F-D6E1-435B-BCDD-7A3149C39A7A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E70">
     <sortCondition ref="C2:C70"/>
   </sortState>
@@ -4081,8 +4111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F26C09-FC50-4613-B0A2-F81A1A868E02}">
   <dimension ref="B2:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5060,10 +5090,18 @@
       </c>
     </row>
     <row r="71" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B71" s="1"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
+      <c r="B71" s="2">
+        <v>69</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="72" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
@@ -5073,9 +5111,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>